<commit_message>
model results updated with ANN, RF updated but no run, SVC no run
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\Desktop\EV-Customer-Discontinuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C0B4029-7229-4816-90D5-A4FF31EE4421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FF4CCA-49CD-44A5-B599-D9CED2C885F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
+    <workbookView xWindow="12953" yWindow="1627" windowWidth="19200" windowHeight="10073" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Pre-processed</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>best parameters</t>
+  </si>
+  <si>
+    <t>u=832, 288, lr=0.001, d=0.05, 0.0</t>
+  </si>
+  <si>
+    <t>u=960, 128, lr=0.01, d=0.5, 0.15</t>
+  </si>
+  <si>
+    <t>u=960, 448, lr=0.01, d=0.0, 0.15</t>
+  </si>
+  <si>
+    <t>96, 96, lr=0.001, d=0.3, 0.1</t>
+  </si>
+  <si>
+    <t>{'C': 10, 'degree': 1, 'gamma': 0.1, 'kernel': 'sigmoid'}</t>
   </si>
 </sst>
 </file>
@@ -107,7 +122,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -288,74 +303,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,13 +698,13 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12.703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.8203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.64453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.76171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.76171875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.29296875" customWidth="1"/>
@@ -703,159 +718,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="23" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A2" s="21"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="22"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
     </row>
     <row r="4" spans="1:15" ht="43" x14ac:dyDescent="0.5">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="15">
         <v>0.73678137776983399</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="15">
         <v>0.52788158648810601</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>0.77869079045909895</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>0.77317108113250099</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>0.76682784966997697</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <v>0.76393012940123906</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="8">
         <v>0.75208932011600205</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="8">
         <v>0.74878759319997801</v>
       </c>
-      <c r="N4" s="17">
+      <c r="N4" s="15">
         <f>MAX(C4,F4,I4,L4)</f>
         <v>0.77869079045909895</v>
       </c>
-      <c r="O4" s="17">
+      <c r="O4" s="15">
         <f>MAX(D4,G4,J4,M4)</f>
         <v>0.77317108113250099</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="18">
         <v>0.73616950000993098</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="18">
         <v>0.52624914090478903</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="17" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="4">
@@ -864,7 +879,7 @@
       <c r="G5" s="3">
         <v>0.85281994703183595</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="17" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="3">
@@ -873,7 +888,7 @@
       <c r="J5" s="4">
         <v>0.85252659960056398</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="17" t="s">
         <v>15</v>
       </c>
       <c r="L5" s="5">
@@ -882,86 +897,104 @@
       <c r="M5" s="5">
         <v>0.84595063358244704</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="18">
         <f t="shared" ref="N5:N8" si="0">MAX(C5,F5,I5,L5)</f>
         <v>0.84562825853999701</v>
       </c>
-      <c r="O5" s="20">
+      <c r="O5" s="18">
         <f t="shared" ref="O5:O8" si="1">MAX(D5,G5,J5,M5)</f>
         <v>0.85281994703183595</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:15" ht="43" x14ac:dyDescent="0.5">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16">
+      <c r="B6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" s="16">
+      <c r="O6" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O7" s="20">
+      <c r="O7" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16">
+      <c r="B8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.72130544106591998</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.70129870129870098</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.65297950763356405</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.71236805824076199</v>
+      </c>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="16">
+        <v>0.72130544106591998</v>
+      </c>
+      <c r="O8" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update Model results xls
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\Desktop\EV-Customer-Discontinuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FF4CCA-49CD-44A5-B599-D9CED2C885F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D05F13-0B3D-45FF-829D-8CDE3884E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12953" yWindow="1627" windowWidth="19200" windowHeight="10073" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -295,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -372,6 +373,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,7 +700,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -999,6 +1001,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="N9" s="26">
+        <f>MAX(N4:N8)</f>
+        <v>0.84562825853999701</v>
+      </c>
+      <c r="O9" s="26">
+        <f>MAX(O4:O8)</f>
+        <v>0.85281994703183595</v>
+      </c>
+    </row>
     <row r="20" spans="10:11" x14ac:dyDescent="0.5">
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1046,4 +1058,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AFE730-3669-401B-AC89-C65E038D7768}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated model results with SVC, and half of RF
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\Desktop\EV-Customer-Discontinuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D05F13-0B3D-45FF-829D-8CDE3884E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5649F3A-30EB-4B80-A645-4E39049D635A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
+    <workbookView xWindow="10940" yWindow="1540" windowWidth="19200" windowHeight="10073" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Pre-processed</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>{'C': 10, 'degree': 1, 'gamma': 0.1, 'kernel': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'C': 100, 'degree': 1, 'gamma': 1, 'kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 15, 'min_samples_leaf': 1, 'min_samples_split': 5, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 30, 'min_samples_leaf': 1, 'min_samples_split': 2, 'n_estimators': 800}</t>
   </si>
 </sst>
 </file>
@@ -352,6 +361,7 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,7 +383,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,7 +709,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -720,57 +729,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="19" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A2" s="22"/>
-      <c r="B2" s="24" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
@@ -807,8 +816,8 @@
       <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
     </row>
     <row r="4" spans="1:15" ht="43" x14ac:dyDescent="0.5">
       <c r="A4" s="12" t="s">
@@ -915,36 +924,70 @@
       <c r="B6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
+      <c r="C6" s="14">
+        <v>0.73863480000652304</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.52853606882422999</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.83169428256074696</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.83573553630159803</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.84100971945423098</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.84548251908156102</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.83373638443577003</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.83994293845344803</v>
+      </c>
       <c r="N6" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.84100971945423098</v>
       </c>
       <c r="O6" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+        <v>0.84548251908156102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
+      <c r="B7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0.73387205387205301</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0.74568926384783096</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.79</v>
+      </c>
       <c r="H7" s="17"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -953,11 +996,11 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.74568926384783096</v>
       </c>
       <c r="O7" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
@@ -1002,11 +1045,11 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="N9" s="26">
+      <c r="N9" s="19">
         <f>MAX(N4:N8)</f>
         <v>0.84562825853999701</v>
       </c>
-      <c r="O9" s="26">
+      <c r="O9" s="19">
         <f>MAX(O4:O8)</f>
         <v>0.85281994703183595</v>
       </c>

</xml_diff>

<commit_message>
modified mode results with RF (upto borderline (incl.))
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\Desktop\EV-Customer-Discontinuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5649F3A-30EB-4B80-A645-4E39049D635A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30A66C0-D56B-4771-8240-BA97C365822A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10940" yWindow="1540" windowWidth="19200" windowHeight="10073" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Pre-processed</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>{'max_depth': 30, 'min_samples_leaf': 1, 'min_samples_split': 2, 'n_estimators': 800}</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>{'max_depth': 15, 'min_samples_leaf': 1, 'min_samples_split': 2, 'n_estimators': 100}</t>
   </si>
 </sst>
 </file>
@@ -305,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -382,6 +388,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -391,8 +415,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDEC8EE"/>
       <color rgb="FFEFE5F7"/>
-      <color rgb="FFDEC8EE"/>
       <color rgb="FFCEAEE6"/>
       <color rgb="FFC39BE1"/>
       <color rgb="FFB381D9"/>
@@ -709,7 +733,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -832,7 +856,7 @@
       <c r="D4" s="15">
         <v>0.52788158648810601</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="27" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="6">
@@ -887,16 +911,16 @@
       <c r="F5" s="4">
         <v>0.84452170790494296</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="4">
         <v>0.85281994703183595</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="32">
         <v>0.84562825853999701</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="32">
         <v>0.85252659960056398</v>
       </c>
       <c r="K5" s="17" t="s">
@@ -939,7 +963,7 @@
       <c r="G6" s="5">
         <v>0.83573553630159803</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="28" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="3">
@@ -974,29 +998,35 @@
         <v>28</v>
       </c>
       <c r="C7" s="18">
-        <v>0.73387205387205301</v>
+        <v>0.762418893861466</v>
       </c>
       <c r="D7" s="18">
         <v>0.8</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="18">
-        <v>0.74568926384783096</v>
-      </c>
-      <c r="G7" s="18">
+      <c r="F7" s="30">
+        <v>0.88586463556529005</v>
+      </c>
+      <c r="G7" s="30">
         <v>0.79</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="H7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.88441665169336103</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.79</v>
+      </c>
       <c r="K7" s="17"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18">
         <f t="shared" si="0"/>
-        <v>0.74568926384783096</v>
+        <v>0.88586463556529005</v>
       </c>
       <c r="O7" s="18">
         <f t="shared" si="1"/>
@@ -1007,34 +1037,42 @@
       <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="3">
         <v>0.72130544106591998</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="5">
         <v>0.70129870129870098</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="H8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="I8" s="14">
         <v>0.65297950763356405</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="K8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="L8" s="4">
         <v>0.71236805824076199</v>
       </c>
-      <c r="M8" s="14"/>
+      <c r="M8" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="N8" s="14">
         <f t="shared" si="0"/>
         <v>0.72130544106591998</v>
@@ -1047,7 +1085,7 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="N9" s="19">
         <f>MAX(N4:N8)</f>
-        <v>0.84562825853999701</v>
+        <v>0.88586463556529005</v>
       </c>
       <c r="O9" s="19">
         <f>MAX(O4:O8)</f>

</xml_diff>

<commit_message>
updated xls with RF grid search results
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\Desktop\EV-Customer-Discontinuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30A66C0-D56B-4771-8240-BA97C365822A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CA86EE-50C0-4172-8ABE-5AC54FC0D89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Pre-processed</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>{'max_depth': 15, 'min_samples_leaf': 1, 'min_samples_split': 2, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 30, 'min_samples_leaf': 1, 'min_samples_split': 2, 'n_estimators': 1200}</t>
   </si>
 </sst>
 </file>
@@ -368,6 +371,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -388,24 +409,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,7 +736,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -753,57 +756,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="20" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="26" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A2" s="23"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25" t="s">
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="24"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
@@ -840,8 +843,8 @@
       <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15" ht="43" x14ac:dyDescent="0.5">
       <c r="A4" s="12" t="s">
@@ -856,7 +859,7 @@
       <c r="D4" s="15">
         <v>0.52788158648810601</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="20" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="6">
@@ -914,13 +917,13 @@
       <c r="G5" s="4">
         <v>0.85281994703183595</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="25">
         <v>0.84562825853999701</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="25">
         <v>0.85252659960056398</v>
       </c>
       <c r="K5" s="17" t="s">
@@ -963,7 +966,7 @@
       <c r="G6" s="5">
         <v>0.83573553630159803</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="21" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="3">
@@ -1003,13 +1006,13 @@
       <c r="D7" s="18">
         <v>0.8</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="23">
         <v>0.88586463556529005</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="23">
         <v>0.79</v>
       </c>
       <c r="H7" s="17" t="s">
@@ -1021,9 +1024,15 @@
       <c r="J7" s="4">
         <v>0.79</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="K7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.875186382568092</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0.79</v>
+      </c>
       <c r="N7" s="18">
         <f t="shared" si="0"/>
         <v>0.88586463556529005</v>
@@ -1037,7 +1046,7 @@
       <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="3">

</xml_diff>

<commit_message>
updated model results with RF fscores
</commit_message>
<xml_diff>
--- a/Model results.xlsx
+++ b/Model results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehna\Desktop\EV-Customer-Discontinuation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CA86EE-50C0-4172-8ABE-5AC54FC0D89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1AF22F-89AD-4573-BD54-E0C6C1356975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{86415F1D-A31A-4F4B-9E3D-42390BA86BE7}"/>
   </bookViews>
@@ -383,12 +383,6 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -409,6 +403,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,7 +736,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -756,57 +756,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="26" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="24" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="27"/>
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31" t="s">
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="30"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
@@ -843,8 +843,8 @@
       <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
     </row>
     <row r="4" spans="1:15" ht="43" x14ac:dyDescent="0.5">
       <c r="A4" s="12" t="s">
@@ -895,7 +895,7 @@
         <v>0.77317108113250099</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" ht="43" x14ac:dyDescent="0.5">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -917,13 +917,13 @@
       <c r="G5" s="4">
         <v>0.85281994703183595</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <v>0.84562825853999701</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="23">
         <v>0.85252659960056398</v>
       </c>
       <c r="K5" s="17" t="s">
@@ -1001,41 +1001,41 @@
         <v>28</v>
       </c>
       <c r="C7" s="18">
-        <v>0.762418893861466</v>
+        <v>0.73387205387205301</v>
       </c>
       <c r="D7" s="18">
         <v>0.8</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="23">
-        <v>0.88586463556529005</v>
-      </c>
-      <c r="G7" s="23">
+      <c r="F7" s="32">
+        <v>0.74568926384783096</v>
+      </c>
+      <c r="G7" s="32">
         <v>0.79</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="4">
-        <v>0.88441665169336103</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="I7" s="3">
+        <v>0.74739281244412603</v>
+      </c>
+      <c r="J7" s="3">
         <v>0.79</v>
       </c>
       <c r="K7" s="17" t="s">
         <v>32</v>
       </c>
       <c r="L7" s="5">
-        <v>0.875186382568092</v>
+        <v>0.74464934178146802</v>
       </c>
       <c r="M7" s="5">
         <v>0.79</v>
       </c>
       <c r="N7" s="18">
         <f t="shared" si="0"/>
-        <v>0.88586463556529005</v>
+        <v>0.74739281244412603</v>
       </c>
       <c r="O7" s="18">
         <f t="shared" si="1"/>
@@ -1094,7 +1094,7 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="N9" s="19">
         <f>MAX(N4:N8)</f>
-        <v>0.88586463556529005</v>
+        <v>0.84562825853999701</v>
       </c>
       <c r="O9" s="19">
         <f>MAX(O4:O8)</f>

</xml_diff>